<commit_message>
Update Homicidios (Ni cuanto commit)
</commit_message>
<xml_diff>
--- a/Homicidios intencionados.xlsx
+++ b/Homicidios intencionados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moises Almanzar\Desktop\Proyecto Samsung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93EDA079-899A-4E74-8E26-18D8AFDF0D4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD984B0-2882-4409-82BC-79705C73F70D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" xr2:uid="{70C545F1-688A-43B5-A908-50A5E78A9D60}"/>
   </bookViews>
@@ -437,7 +437,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="B2" sqref="B2:D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -470,13 +470,13 @@
         <v>2022</v>
       </c>
       <c r="B2" s="1">
-        <v>1.389</v>
+        <v>1389</v>
       </c>
       <c r="C2" s="1">
         <v>153</v>
       </c>
       <c r="D2" s="1">
-        <v>1.236</v>
+        <v>1236</v>
       </c>
       <c r="E2" s="1">
         <v>90</v>
@@ -493,13 +493,13 @@
         <v>2021</v>
       </c>
       <c r="B3" s="1">
-        <v>1.1719999999999999</v>
+        <v>1172</v>
       </c>
       <c r="C3" s="1">
         <v>142</v>
       </c>
       <c r="D3" s="1">
-        <v>1.03</v>
+        <v>103</v>
       </c>
       <c r="E3" s="1">
         <v>90</v>
@@ -539,7 +539,7 @@
         <v>2019</v>
       </c>
       <c r="B5" s="1">
-        <v>1.026</v>
+        <v>1026</v>
       </c>
       <c r="C5" s="1">
         <v>145</v>
@@ -562,7 +562,7 @@
         <v>2018</v>
       </c>
       <c r="B6" s="1">
-        <v>1.0680000000000001</v>
+        <v>1068</v>
       </c>
       <c r="C6" s="1">
         <v>152</v>
@@ -585,13 +585,13 @@
         <v>2017</v>
       </c>
       <c r="B7" s="1">
-        <v>1.216</v>
+        <v>1216</v>
       </c>
       <c r="C7" s="1">
         <v>191</v>
       </c>
       <c r="D7" s="1">
-        <v>1.0249999999999999</v>
+        <v>1025</v>
       </c>
       <c r="E7" s="1">
         <v>115</v>
@@ -608,13 +608,13 @@
         <v>2016</v>
       </c>
       <c r="B8" s="1">
-        <v>1.6160000000000001</v>
+        <v>1616</v>
       </c>
       <c r="C8" s="1">
         <v>170</v>
       </c>
       <c r="D8" s="1">
-        <v>1.446</v>
+        <v>1446</v>
       </c>
       <c r="E8" s="1">
         <v>84</v>
@@ -631,13 +631,13 @@
         <v>2014</v>
       </c>
       <c r="B9" s="1">
-        <v>1.81</v>
+        <v>181</v>
       </c>
       <c r="C9" s="1">
         <v>187</v>
       </c>
       <c r="D9" s="1">
-        <v>1.623</v>
+        <v>1623</v>
       </c>
       <c r="E9" s="1">
         <v>0</v>
@@ -654,7 +654,7 @@
         <v>2013</v>
       </c>
       <c r="B10" s="1">
-        <v>1.978</v>
+        <v>1978</v>
       </c>
       <c r="C10" s="1">
         <v>0</v>
@@ -677,13 +677,13 @@
         <v>2012</v>
       </c>
       <c r="B11" s="1">
-        <v>2.2679999999999998</v>
+        <v>2268</v>
       </c>
       <c r="C11" s="1">
         <v>201</v>
       </c>
       <c r="D11" s="1">
-        <v>2.0670000000000002</v>
+        <v>2067</v>
       </c>
       <c r="E11" s="1">
         <v>0</v>
@@ -700,13 +700,13 @@
         <v>2011</v>
       </c>
       <c r="B12" s="1">
-        <v>2.5129999999999999</v>
+        <v>2513</v>
       </c>
       <c r="C12" s="1">
         <v>233</v>
       </c>
       <c r="D12" s="1">
-        <v>2.2799999999999998</v>
+        <v>228</v>
       </c>
       <c r="E12" s="1">
         <v>83</v>
@@ -723,13 +723,13 @@
         <v>2010</v>
       </c>
       <c r="B13" s="1">
-        <v>2.4740000000000002</v>
+        <v>2474</v>
       </c>
       <c r="C13" s="1">
         <v>210</v>
       </c>
       <c r="D13" s="1">
-        <v>2.2639999999999998</v>
+        <v>2264</v>
       </c>
       <c r="E13" s="1">
         <v>65</v>
@@ -746,13 +746,13 @@
         <v>2009</v>
       </c>
       <c r="B14" s="1">
-        <v>2.375</v>
+        <v>2375</v>
       </c>
       <c r="C14" s="1">
         <v>180</v>
       </c>
       <c r="D14" s="1">
-        <v>2.1949999999999998</v>
+        <v>2195</v>
       </c>
       <c r="E14" s="1">
         <v>54</v>
@@ -769,13 +769,13 @@
         <v>2008</v>
       </c>
       <c r="B15" s="1">
-        <v>2.3940000000000001</v>
+        <v>2394</v>
       </c>
       <c r="C15" s="1">
         <v>187</v>
       </c>
       <c r="D15" s="1">
-        <v>2.2069999999999999</v>
+        <v>2207</v>
       </c>
       <c r="E15" s="1">
         <v>0</v>
@@ -792,13 +792,13 @@
         <v>2007</v>
       </c>
       <c r="B16" s="1">
-        <v>2.1110000000000002</v>
+        <v>2111</v>
       </c>
       <c r="C16" s="1">
         <v>175</v>
       </c>
       <c r="D16" s="1">
-        <v>1.9359999999999999</v>
+        <v>1936</v>
       </c>
       <c r="E16" s="1">
         <v>0</v>
@@ -815,13 +815,13 @@
         <v>2006</v>
       </c>
       <c r="B17" s="1">
-        <v>2.1440000000000001</v>
+        <v>2144</v>
       </c>
       <c r="C17" s="1">
         <v>180</v>
       </c>
       <c r="D17" s="1">
-        <v>1.964</v>
+        <v>1964</v>
       </c>
       <c r="E17" s="1">
         <v>0</v>
@@ -838,13 +838,13 @@
         <v>2005</v>
       </c>
       <c r="B18" s="1">
-        <v>2.3940000000000001</v>
+        <v>2394</v>
       </c>
       <c r="C18" s="1">
         <v>214</v>
       </c>
       <c r="D18" s="1">
-        <v>2.1800000000000002</v>
+        <v>218</v>
       </c>
       <c r="E18" s="1">
         <v>0</v>
@@ -861,7 +861,7 @@
         <v>2004</v>
       </c>
       <c r="B19" s="1">
-        <v>2.2389999999999999</v>
+        <v>2239</v>
       </c>
       <c r="C19" s="1">
         <v>0</v>
@@ -884,7 +884,7 @@
         <v>2003</v>
       </c>
       <c r="B20" s="1">
-        <v>1.9019999999999999</v>
+        <v>1902</v>
       </c>
       <c r="C20" s="1">
         <v>0</v>
@@ -907,7 +907,7 @@
         <v>2002</v>
       </c>
       <c r="B21" s="1">
-        <v>1.2789999999999999</v>
+        <v>1279</v>
       </c>
       <c r="C21" s="1">
         <v>0</v>
@@ -930,7 +930,7 @@
         <v>2001</v>
       </c>
       <c r="B22" s="1">
-        <v>1.095</v>
+        <v>1095</v>
       </c>
       <c r="C22" s="1">
         <v>0</v>
@@ -953,7 +953,7 @@
         <v>2000</v>
       </c>
       <c r="B23" s="1">
-        <v>1.21</v>
+        <v>121</v>
       </c>
       <c r="C23" s="1">
         <v>0</v>
@@ -976,7 +976,7 @@
         <v>1999</v>
       </c>
       <c r="B24" s="1">
-        <v>1.0660000000000001</v>
+        <v>1066</v>
       </c>
       <c r="C24" s="1">
         <v>0</v>
@@ -999,7 +999,7 @@
         <v>1998</v>
       </c>
       <c r="B25" s="1">
-        <v>1.121</v>
+        <v>1121</v>
       </c>
       <c r="C25" s="1">
         <v>0</v>
@@ -1022,7 +1022,7 @@
         <v>1997</v>
       </c>
       <c r="B26" s="1">
-        <v>1.038</v>
+        <v>1038</v>
       </c>
       <c r="C26" s="1">
         <v>0</v>
@@ -1045,7 +1045,7 @@
         <v>1996</v>
       </c>
       <c r="B27" s="1">
-        <v>1.032</v>
+        <v>1032</v>
       </c>
       <c r="C27" s="1">
         <v>0</v>
@@ -1068,7 +1068,7 @@
         <v>1995</v>
       </c>
       <c r="B28" s="1">
-        <v>1.0069999999999999</v>
+        <v>1007</v>
       </c>
       <c r="C28" s="1">
         <v>0</v>
@@ -1091,7 +1091,7 @@
         <v>1994</v>
       </c>
       <c r="B29" s="1">
-        <v>1.0049999999999999</v>
+        <v>1005</v>
       </c>
       <c r="C29" s="1">
         <v>0</v>

</xml_diff>

<commit_message>
Otro commit ma, la semilla
</commit_message>
<xml_diff>
--- a/Homicidios intencionados.xlsx
+++ b/Homicidios intencionados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moises Almanzar\Desktop\Proyecto Samsung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD984B0-2882-4409-82BC-79705C73F70D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20AF0B94-2216-4412-8143-CACA6139990A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" xr2:uid="{70C545F1-688A-43B5-A908-50A5E78A9D60}"/>
   </bookViews>
@@ -437,7 +437,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D32"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -631,7 +631,7 @@
         <v>2014</v>
       </c>
       <c r="B9" s="1">
-        <v>181</v>
+        <v>1810</v>
       </c>
       <c r="C9" s="1">
         <v>187</v>
@@ -953,7 +953,7 @@
         <v>2000</v>
       </c>
       <c r="B23" s="1">
-        <v>121</v>
+        <v>1210</v>
       </c>
       <c r="C23" s="1">
         <v>0</v>

</xml_diff>